<commit_message>
Filled out section 6.5.3 from the RFP in a new wheet
</commit_message>
<xml_diff>
--- a/ReferenceDocuments/Requirements.xlsx
+++ b/ReferenceDocuments/Requirements.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
+    <sheet name="RFP Requirements" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="260">
   <si>
     <t>Table 1</t>
   </si>
@@ -2024,6 +2025,294 @@
         <rFont val="Helvetica"/>
       </rPr>
       <t xml:space="preserve"> information that would not be present in an unconstrained model</t>
+    </r>
+  </si>
+  <si>
+    <t>6.5.2 Reference Model Requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.5.2.1 Submissions shall support the ability to model the relationships between archetype model elements (AME) and the reference model elements (RME) from which they are defined. </t>
+  </si>
+  <si>
+    <t>The RMP defines the &lt;&lt;ReferenceModel&gt;&gt; stereotype which identifies a package in the reference model that directly or indirectly contains the set of classes that can be constrained by AME’s.  The CMP requires that (a) an &lt;&lt;ArchetypeLibrary&gt;&gt; package import a &lt;&lt;ReferenceModel&gt;&gt; package (b)all &lt;&lt;Archetype&gt;&gt; packages must be contained in an &lt;&lt;ArchetypeLibrary&gt;&gt;, (c) that a &lt;&lt;ArchetypeVersion&gt;&gt; classifiers constrain a classifier that is contained in the &lt;&lt;ReferenceModel&gt;&gt; package.  An “AME” in the CMP context is defined as any Classifier that is stereotyped by a specialization of &lt;&lt;ObjectConstraint&gt;&gt;.  An &lt;&lt;ArchetypeVersion&gt;&gt; must be a &lt;&lt;ComplexObjectConstraint&gt;&gt; which is a type of &lt;&lt;ObjectConstraint&gt;&gt;, and all &lt;&lt;ArchetypeVersions&gt;&gt; must specialize a classifier with an ancestor that is owned by the &lt;&lt;ReferenceModel&gt;&gt; package.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.5.2.2 Submissions shall support the ability of each archetype model element (AME) to be associated with progenitor model elements. </t>
+  </si>
+  <si>
+    <t>The &lt;&lt;Constrains&gt;&gt; stereotype extends Generalization and requires that the specific end of must be a classifier stereotyped by &lt;&lt;ObjectConstraint&gt;&gt;.  This means that all but the “topmost” ObjectConstraint is an AMI.</t>
+  </si>
+  <si>
+    <t>6.5.2.3 Submissions shall support the ability of each archetype model element to be directly or indirectly (through subsetting) extended from a single meta element, which contains all the tags/properties required by all archetype model elements.  Submissions shall substantiate properties chosen.</t>
+  </si>
+  <si>
+    <t>The choice of the single “meta element” is left to the reference model itself.  A reference model, if it so chooses, may have all model classes descend from a root class.  As an example, the CIMI Reference Model Version 3.0.1 [cite: CRM 3.0.1] derives all model elements from the LOCATABLE class.   + +The AML specification allows but does not require the presence of any tags or properties that must be common to all model elements.  The RMP does, however, allow reference model properties to be stereotyped as &lt;&lt;Infrastructure&gt;&gt; and &lt;&lt;Runtime&gt;&gt; properties that identify them as properties that are associated with instance identification and provenance respectively.</t>
+  </si>
+  <si>
+    <t>6.5.2.4 Submission shall provide a set of primitive data types. Example types such as the following are included for consideration (Integer, Real, Boolean, Character, String, Date, Time, DateTime and Duration)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">Section 8.2.2 AML Data Types identifies the set of “Primitive” data types that are supported by the AML profile.  They include everything in the suggested set with the exception of </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>Character</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>, as there were no known examples or use cases for this within CIMI or the AML 1.5/2.0 specifications.  AML did add one additional “primitive” data type, TerminologyCode</t>
+    </r>
+  </si>
+  <si>
+    <t>6.5.3.4 Submissions shall provide the ability for differential representation of archetype Models (AMs)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">With one exception, the UML generalization / specialization model supports this “out of the box”.  The one exception is multiplicity, where the UML specification states that lower or upper values that are not explicitly stated have default values.  The AML specification requires that lower and/or upper values should not be stated </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>unless</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> they are different from the inherited values.</t>
+    </r>
+  </si>
+  <si>
+    <t>6.5.3.5 Submissions shall provide a flattening specification.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">This ability is built in to the UML model, where any specialization includes all constraints that are inherited from its general ancestors.  The ability to </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>display</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> this information is the function of a modeling tool.  The UML “ownedMember”  and related “owned” properties identify the differential form and the “member” and related properties the flattening / aggregation.</t>
+    </r>
+  </si>
+  <si>
+    <t>6.5.3.6 Submissions shall provide the ability to capture and maintain tractable lineage from flattened to progenitor AM’s</t>
+  </si>
+  <si>
+    <t>This ability is inherent in the UML metamodel, as the “progenitor” classes are never removed in the flattening process — flattening is only a view on the same internal infrastructure.</t>
+  </si>
+  <si>
+    <t>6.5.3.7 Submissions shall provide the ability for an AM to be re-used by another AM by direct reference.</t>
+  </si>
+  <si>
+    <t>This is accomplished by the UML import mechanism, where an AM (a package stereotyped by &lt;&lt;Archetype&gt;&gt;) may be imported into another &lt;&lt;Archetype&gt;&gt; package.</t>
+  </si>
+  <si>
+    <t>6.5.3.8  Submissions shall provide the ability for an AM to be composed from a set of other pre-existing AM’s</t>
+  </si>
+  <si>
+    <t>The &lt;&lt;ArchetypeRootProxy&gt;&gt; constraint allows the specification of a “slot” that can be filled by any ArchetypeVersion that constrains the same target reference model class.</t>
+  </si>
+  <si>
+    <t>6.5.3.9  Submission shall allow model elements within an AM to be constrained to a given Reference Model class subtype.</t>
+  </si>
+  <si>
+    <t>This ability is accomplished by the UML property redefinition and subsetting mechanisms, where the types of redefined or subsetted properties can be filled with instances of a given classifier or any specialization thereof.</t>
+  </si>
+  <si>
+    <t>6.5.3.10 Submission shall provide the ability in an AM to constrain RM attributes to a given [primitive] type and to specify a valid value set.</t>
+  </si>
+  <si>
+    <t>The specializations of the &lt;&lt;PrimitiveObjectConstraint&gt;&gt; stereotype allow the specification of sets of possible values,  sets of value ranges, match patterns where appropriate.</t>
+  </si>
+  <si>
+    <t>6.5.3.11 Submissions shall provide the ability to provide default and assumed values for AM elements of both primitive and complex types.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">The ADL 2.0 specification [cite: ADL2.0] states “[Default values are] almost always limited to use in templates, since default values are usually specific to local contexts or use cases,” and their primary purpose is to inform instance constructors of the preferred/only value to fill in when creating a new classifier instance.   This was determined to be out of scope for the current AML profile, as its focus was on expressing static constraints and not on how the construction of object instances actually occurred.  That said, one interpretation of the UML </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>default</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> property could be to accomplish this purpose, meaning that AML developers aren’t precluded from using this where required. + +The AML specification has (reluctantly) included the ability to specify an assumed value for any classifier constrained by the &lt;&lt;PrimitiveObjectConstraint&gt;&gt; stereotype.  We say “reluctantly” because assumed values violate one of the fundamental premises underlying the AML specification itself — that instances of the general, unconstrained classifier are always valid instance of the those that comply with the constraint.   If the constraint provides additional values that aren’t present in the general model, this might result in some serious problems down the line. + +The AML specification does </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> specify the ability to directly provide assumed values for complex types, as the set of use cases is limited and those we did encounter could be addressed with collections of “primitive” (AML data type) assumed values.</t>
+    </r>
+  </si>
+  <si>
+    <t>6.5.3.12 Submissions shall provide the ability to specify the allowable occurrence[s] of instance data.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">The UML </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>subsets</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> property attribute allows multiple partitions of the same parent property, each with their own minimum and/or maximum occurrences.  The UML </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">subsets </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>semantics do not allow impossible situations to be specified.  See: 6.5.3.13 below for details.</t>
+    </r>
+  </si>
+  <si>
+    <t>6.5.3.13 Submission shall provide the ability to define cardinality that is subsumed by progenitor elements.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">The UML </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>redefines</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>subsets</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> property attributes provide this ability natively. Subsetting allows the upper multiplicity of a property to be restricted to any value less than the the current maximum, including “0”, meaning that an optional value cannot be present.  It also allows lower values to be increased meaning that optional values can be made mandatory.</t>
     </r>
   </si>
 </sst>
@@ -2169,7 +2458,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2240,6 +2529,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3502,7 +3797,7 @@
   <sheetFormatPr defaultColWidth="9.03" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="11.6328" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.8359" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.4375" style="1" customWidth="1"/>
     <col min="3" max="3" width="28.7031" style="1" customWidth="1"/>
     <col min="4" max="4" width="28.7031" style="1" customWidth="1"/>
     <col min="5" max="5" width="25.1484" style="1" customWidth="1"/>
@@ -3550,7 +3845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" ht="57.85" customHeight="1">
+    <row r="3" ht="45.85" customHeight="1">
       <c r="A3" t="s" s="4">
         <v>7</v>
       </c>
@@ -4787,4 +5082,223 @@
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="C3" xSplit="2" ySplit="2" activePane="bottomRight" state="frozenSplit"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="0.25" style="24" customWidth="1"/>
+    <col min="2" max="2" width="12.25" style="24" customWidth="1"/>
+    <col min="3" max="3" width="12.25" style="24" customWidth="1"/>
+    <col min="4" max="4" width="34.8203" style="24" customWidth="1"/>
+    <col min="5" max="5" width="12.25" style="24" customWidth="1"/>
+    <col min="6" max="6" width="12.25" style="24" customWidth="1"/>
+    <col min="7" max="7" width="12.25" style="24" customWidth="1"/>
+    <col min="8" max="256" width="12.25" style="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="2" customHeight="1"/>
+    <row r="2" ht="20.55" customHeight="1">
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+    </row>
+    <row r="3" ht="44.55" customHeight="1">
+      <c r="B3" t="s" s="12">
+        <v>231</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" ht="200.35" customHeight="1">
+      <c r="B4" s="9"/>
+      <c r="C4" t="s" s="10">
+        <v>232</v>
+      </c>
+      <c r="D4" t="s" s="10">
+        <v>233</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" ht="116.35" customHeight="1">
+      <c r="B5" s="9"/>
+      <c r="C5" t="s" s="10">
+        <v>234</v>
+      </c>
+      <c r="D5" t="s" s="10">
+        <v>235</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" ht="236.35" customHeight="1">
+      <c r="B6" s="9"/>
+      <c r="C6" t="s" s="10">
+        <v>236</v>
+      </c>
+      <c r="D6" t="s" s="10">
+        <v>237</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" ht="164.35" customHeight="1">
+      <c r="B7" s="9"/>
+      <c r="C7" t="s" s="10">
+        <v>238</v>
+      </c>
+      <c r="D7" t="s" s="10">
+        <v>239</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" ht="92.35" customHeight="1">
+      <c r="B8" s="9"/>
+      <c r="C8" t="s" s="10">
+        <v>240</v>
+      </c>
+      <c r="D8" t="s" s="10">
+        <v>241</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" ht="92.35" customHeight="1">
+      <c r="B9" s="9"/>
+      <c r="C9" t="s" s="10">
+        <v>242</v>
+      </c>
+      <c r="D9" t="s" s="10">
+        <v>243</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" ht="104.35" customHeight="1">
+      <c r="B10" s="9"/>
+      <c r="C10" t="s" s="10">
+        <v>244</v>
+      </c>
+      <c r="D10" t="s" s="10">
+        <v>245</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" ht="80.35" customHeight="1">
+      <c r="B11" s="9"/>
+      <c r="C11" t="s" s="10">
+        <v>246</v>
+      </c>
+      <c r="D11" t="s" s="10">
+        <v>247</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+    </row>
+    <row r="12" ht="92.35" customHeight="1">
+      <c r="B12" s="9"/>
+      <c r="C12" t="s" s="10">
+        <v>248</v>
+      </c>
+      <c r="D12" t="s" s="10">
+        <v>249</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+    </row>
+    <row r="13" ht="104.35" customHeight="1">
+      <c r="B13" s="9"/>
+      <c r="C13" t="s" s="10">
+        <v>250</v>
+      </c>
+      <c r="D13" t="s" s="10">
+        <v>251</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+    </row>
+    <row r="14" ht="104.35" customHeight="1">
+      <c r="B14" s="9"/>
+      <c r="C14" t="s" s="10">
+        <v>252</v>
+      </c>
+      <c r="D14" t="s" s="10">
+        <v>253</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" ht="356.35" customHeight="1">
+      <c r="B15" s="9"/>
+      <c r="C15" t="s" s="10">
+        <v>254</v>
+      </c>
+      <c r="D15" t="s" s="10">
+        <v>255</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" ht="92.35" customHeight="1">
+      <c r="B16" s="9"/>
+      <c r="C16" t="s" s="10">
+        <v>256</v>
+      </c>
+      <c r="D16" t="s" s="10">
+        <v>257</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" ht="92.35" customHeight="1">
+      <c r="B17" s="9"/>
+      <c r="C17" t="s" s="10">
+        <v>258</v>
+      </c>
+      <c r="D17" t="s" s="10">
+        <v>259</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>